<commit_message>
service analisis cluster update
</commit_message>
<xml_diff>
--- a/services/risk_dimensions.xlsx
+++ b/services/risk_dimensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roise\Documents\Apam ciber\leaks\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E97DCE-9236-467D-9D86-23F2FC0E03C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0FDB7E-EBD8-485F-9283-9E1C750BA25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,15 +18,10 @@
     <sheet name="Privacy values" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Services clean'!#REF!</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Services clean'!#REF!</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Services clean'!#REF!</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Services clean'!$AB$2:$AB$76</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Services test'!$AC$2:$AC$76</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Services test'!$AD$2:$AD$76</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Services test'!$AE$2:$AE$76</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Services test'!$AD$2:$AD$76</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Services test'!$AF$2:$AF$76</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Services test'!$AD$2:$AD$76</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Services test'!$AE$2:$AE$76</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Services test'!$AC$2:$AC$76</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Services test'!$AF$2:$AF$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -981,7 +976,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -991,9 +986,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="4"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
@@ -1023,6 +1017,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1091,7 +1086,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1179,7 +1173,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1240,7 +1234,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1301,7 +1295,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1362,7 +1356,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3933,7 +3927,7 @@
     <sortCondition ref="C1:C76"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{071B4CFE-A03A-4AF7-B42B-C2B7DAA07DCB}" name="Website" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{071B4CFE-A03A-4AF7-B42B-C2B7DAA07DCB}" name="Website" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{028F8BBD-31E2-4672-93E2-F1D5B57B06E7}" name="Domain name"/>
     <tableColumn id="3" xr3:uid="{495839F7-72B2-4D33-B257-D25EE0AF3720}" name="Type"/>
     <tableColumn id="4" xr3:uid="{0A72491A-C0F4-4953-B010-2D1A2CFF0B67}" name="Company"/>
@@ -3957,9 +3951,9 @@
     <tableColumn id="19" xr3:uid="{2F9AFFDC-06F4-46CE-8B09-1E3AB11FB27F}" name="Messages"/>
     <tableColumn id="20" xr3:uid="{CC102357-8ABD-4B62-9A2C-8615EA74B057}" name="subscription"/>
     <tableColumn id="21" xr3:uid="{9A8F6B4C-580A-454D-A45F-531D0093D8CB}" name="purchases"/>
-    <tableColumn id="24" xr3:uid="{BC1D07B0-AB2C-44CA-B95E-0914F2FB83EE}" name="money stored" dataDxfId="2"/>
-    <tableColumn id="25" xr3:uid="{171EEF98-D3DA-4D14-A89F-D2327B05271C}" name="key to other accounts" dataDxfId="1"/>
-    <tableColumn id="29" xr3:uid="{964289FB-1944-470B-AF80-DED834E4EBD0}" name="Sexual preferences" dataDxfId="0"/>
+    <tableColumn id="24" xr3:uid="{BC1D07B0-AB2C-44CA-B95E-0914F2FB83EE}" name="money stored" dataDxfId="7"/>
+    <tableColumn id="25" xr3:uid="{171EEF98-D3DA-4D14-A89F-D2327B05271C}" name="key to other accounts" dataDxfId="6"/>
+    <tableColumn id="29" xr3:uid="{964289FB-1944-470B-AF80-DED834E4EBD0}" name="Sexual preferences" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3971,7 +3965,7 @@
     <sortCondition ref="C1:C76"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{D49D63F5-14C4-474F-AC2A-717807CBA19D}" name="Website" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{D49D63F5-14C4-474F-AC2A-717807CBA19D}" name="Website" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{967C92E5-930D-421B-96AB-24880DF56001}" name="Domain name"/>
     <tableColumn id="3" xr3:uid="{0F98C143-4D0B-4475-9B66-A3B7B357676B}" name="Type"/>
     <tableColumn id="4" xr3:uid="{FE726D90-FE6D-45AE-A82B-74913D74B4C9}" name="Company"/>
@@ -3995,10 +3989,10 @@
     <tableColumn id="19" xr3:uid="{6D279B90-8B6A-4969-AA25-549CB632101F}" name="Messages"/>
     <tableColumn id="20" xr3:uid="{ED04A4C0-FB40-44A6-83DA-2CC6D398451E}" name="subscription"/>
     <tableColumn id="21" xr3:uid="{E5146E0C-0CB1-4A72-8CC4-D894B22246AB}" name="purchases"/>
-    <tableColumn id="24" xr3:uid="{B3AA793D-C1A7-4FEF-9806-0EBB14D673EF}" name="money stored" dataDxfId="7"/>
-    <tableColumn id="25" xr3:uid="{65983C56-E6B3-4E44-9E39-FF5DD8D46B16}" name="key to other accounts" dataDxfId="6"/>
-    <tableColumn id="29" xr3:uid="{FAC1B20E-7929-44D8-BCF3-FA3836B357D2}" name="Sexual preferences" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{75CC30E7-C3D3-415D-B891-9ACAF13E6392}" name="risk" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{B3AA793D-C1A7-4FEF-9806-0EBB14D673EF}" name="money stored" dataDxfId="3"/>
+    <tableColumn id="25" xr3:uid="{65983C56-E6B3-4E44-9E39-FF5DD8D46B16}" name="key to other accounts" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{FAC1B20E-7929-44D8-BCF3-FA3836B357D2}" name="Sexual preferences" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{75CC30E7-C3D3-415D-B891-9ACAF13E6392}" name="risk" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7833,7 +7827,7 @@
     <row r="87" spans="28:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="88" spans="28:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="89" spans="28:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AB89" s="13"/>
+      <c r="AB89" s="12"/>
     </row>
     <row r="90" spans="28:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="28:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13065,26 +13059,22 @@
       </c>
     </row>
     <row r="77" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="9"/>
-      <c r="Y77" s="9"/>
-      <c r="Z77" s="9"/>
-      <c r="AA77" s="9"/>
       <c r="AB77" t="s">
         <v>232</v>
       </c>
-      <c r="AC77" s="10">
+      <c r="AC77" s="9">
         <f>MAX(AC2:AC76)</f>
         <v>13.466862431914784</v>
       </c>
-      <c r="AD77" s="10">
+      <c r="AD77" s="9">
         <f t="shared" ref="AD77:AF77" si="0">MAX(AD2:AD76)</f>
         <v>101</v>
       </c>
-      <c r="AE77" s="10">
+      <c r="AE77" s="9">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AF77" s="10">
+      <c r="AF77" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -13169,19 +13159,19 @@
       <c r="AB78" t="s">
         <v>234</v>
       </c>
-      <c r="AC78" s="10">
+      <c r="AC78" s="9">
         <f>MIN(AC2:AC76)</f>
         <v>1.2190136542044754</v>
       </c>
-      <c r="AD78" s="10">
+      <c r="AD78" s="9">
         <f t="shared" ref="AD78:AF78" si="1">MIN(AD2:AD76)</f>
         <v>9</v>
       </c>
-      <c r="AE78" s="10">
+      <c r="AE78" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="AF78" s="10">
+      <c r="AF78" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -13266,19 +13256,19 @@
       <c r="AB79" t="s">
         <v>26</v>
       </c>
-      <c r="AC79" s="10">
+      <c r="AC79" s="9">
         <f>GEOMEAN(AC2:AC76)</f>
         <v>7.0051105610094488</v>
       </c>
-      <c r="AD79" s="10">
+      <c r="AD79" s="9">
         <f t="shared" ref="AD79:AF79" si="2">GEOMEAN(AD2:AD76)</f>
         <v>52.286969945621912</v>
       </c>
-      <c r="AE79" s="10">
+      <c r="AE79" s="9">
         <f t="shared" si="2"/>
         <v>12.068861269491313</v>
       </c>
-      <c r="AF79" s="10">
+      <c r="AF79" s="9">
         <f t="shared" si="2"/>
         <v>6.7264063004347427</v>
       </c>
@@ -13363,19 +13353,19 @@
       <c r="AB80" t="s">
         <v>233</v>
       </c>
-      <c r="AC80" s="10">
+      <c r="AC80" s="9">
         <f>MEDIAN(AC5:AC79)</f>
         <v>7.5930249580565441</v>
       </c>
-      <c r="AD80" s="10">
+      <c r="AD80" s="9">
         <f t="shared" ref="AD80:AF80" si="3">MEDIAN(AD5:AD79)</f>
         <v>56</v>
       </c>
-      <c r="AE80" s="10">
+      <c r="AE80" s="9">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="AF80" s="10">
+      <c r="AF80" s="9">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -13460,19 +13450,19 @@
       <c r="AB81" t="s">
         <v>235</v>
       </c>
-      <c r="AC81" s="10">
+      <c r="AC81" s="9">
         <f>_xlfn.STDEV.P(AC6:AC80)</f>
         <v>2.9348849365101399</v>
       </c>
-      <c r="AD81" s="10">
+      <c r="AD81" s="9">
         <f t="shared" ref="AD81:AF81" si="4">_xlfn.STDEV.P(AD6:AD80)</f>
         <v>22.034778230727433</v>
       </c>
-      <c r="AE81" s="10">
+      <c r="AE81" s="9">
         <f t="shared" si="4"/>
         <v>5.1775469626384893</v>
       </c>
-      <c r="AF81" s="10">
+      <c r="AF81" s="9">
         <f t="shared" si="4"/>
         <v>3.0917587614646056</v>
       </c>
@@ -13482,19 +13472,19 @@
       <c r="AB83" t="s">
         <v>237</v>
       </c>
-      <c r="AC83" s="12">
+      <c r="AC83" s="11">
         <f>SUM(J78:AA78)</f>
         <v>25.987754751789382</v>
       </c>
-      <c r="AD83" s="12">
+      <c r="AD83" s="11">
         <f>SUM(J79:AA79)</f>
         <v>194</v>
       </c>
-      <c r="AE83" s="12">
+      <c r="AE83" s="11">
         <f>SUM(J80:AA80)</f>
         <v>44</v>
       </c>
-      <c r="AF83" s="12">
+      <c r="AF83" s="11">
         <f>SUM(J81:AA81)</f>
         <v>27</v>
       </c>
@@ -13538,7 +13528,7 @@
       <c r="AB90" t="s">
         <v>243</v>
       </c>
-      <c r="AD90" s="13" t="s">
+      <c r="AD90" s="12" t="s">
         <v>248</v>
       </c>
     </row>
@@ -14596,7 +14586,7 @@
       <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="11"/>
+      <c r="T1" s="10"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
services analisis radar and final changes
</commit_message>
<xml_diff>
--- a/services/risk_dimensions.xlsx
+++ b/services/risk_dimensions.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roise\Documents\Apam ciber\leaks\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0FDB7E-EBD8-485F-9283-9E1C750BA25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88360280-C6FF-4413-86C0-A00E114BEF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Services clean" sheetId="4" r:id="rId1"/>
-    <sheet name="Services test" sheetId="3" r:id="rId2"/>
-    <sheet name="Privacy values" sheetId="1" r:id="rId3"/>
+    <sheet name="privacy values clean" sheetId="5" r:id="rId2"/>
+    <sheet name="Services test" sheetId="3" r:id="rId3"/>
+    <sheet name="Privacy values" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Services test'!$AD$2:$AD$76</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Services test'!$AE$2:$AE$76</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Services test'!$AE$2:$AE$76</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Services test'!$AD$2:$AD$76</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Services test'!$AC$2:$AC$76</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Services test'!$AF$2:$AF$76</definedName>
   </definedNames>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="252">
   <si>
     <t>Nickname</t>
   </si>
@@ -1234,7 +1235,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1295,7 +1296,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4263,8 +4264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C522F9-F455-4B38-A565-C6DB8983C156}">
   <dimension ref="A1:AB988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AB2" sqref="AB2"/>
@@ -8750,6 +8751,493 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E52125-0BEB-4F52-AF5D-6A00A0E48DCD}">
+  <dimension ref="A1:S8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>4</v>
+      </c>
+      <c r="Q4">
+        <v>4</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F9EBD0-2CFC-417B-A678-6B092CE088D1}">
   <dimension ref="A1:AF989"/>
   <sheetViews>
@@ -14515,12 +15003,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection sqref="A1:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new plots for services
</commit_message>
<xml_diff>
--- a/services/risk_dimensions.xlsx
+++ b/services/risk_dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roise\Documents\Apam ciber\leaks\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88360280-C6FF-4413-86C0-A00E114BEF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9485C6B7-E3D7-4F37-9F9F-F31F809AFCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Services clean" sheetId="4" r:id="rId1"/>
@@ -19,10 +19,10 @@
     <sheet name="Privacy values" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Services test'!$AE$2:$AE$76</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Services test'!$AC$2:$AC$76</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'Services test'!$AD$2:$AD$76</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Services test'!$AC$2:$AC$76</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Services test'!$AF$2:$AF$76</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Services test'!$AF$2:$AF$76</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Services test'!$AE$2:$AE$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -782,25 +782,25 @@
     <t>very high</t>
   </si>
   <si>
-    <t>0-20</t>
-  </si>
-  <si>
-    <t>20-40</t>
-  </si>
-  <si>
-    <t>40-60</t>
-  </si>
-  <si>
-    <t>60-80</t>
-  </si>
-  <si>
-    <t>80-100</t>
-  </si>
-  <si>
     <t>death</t>
   </si>
   <si>
-    <t>100-</t>
+    <t>0-30</t>
+  </si>
+  <si>
+    <t>30-60</t>
+  </si>
+  <si>
+    <t>60-90</t>
+  </si>
+  <si>
+    <t>90-120</t>
+  </si>
+  <si>
+    <t>120-150</t>
+  </si>
+  <si>
+    <t>150-</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1174,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1296,7 +1296,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1357,7 +1357,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4264,11 +4264,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C522F9-F455-4B38-A565-C6DB8983C156}">
   <dimension ref="A1:AB988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F57" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB2" sqref="AB2"/>
+      <selection pane="bottomRight" activeCell="C36" sqref="C36:AB37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="AB2" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>65</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -4474,7 +4474,7 @@
       </c>
       <c r="AB3" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>64</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -4516,7 +4516,7 @@
       </c>
       <c r="AB4" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>57</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -4564,7 +4564,7 @@
       </c>
       <c r="AB5" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>72</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -4618,7 +4618,7 @@
       </c>
       <c r="AB6" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>72</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -4672,7 +4672,7 @@
       </c>
       <c r="AB7" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>100</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -4699,7 +4699,7 @@
       </c>
       <c r="AB8" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -4741,7 +4741,7 @@
       </c>
       <c r="AB9" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>79</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -4768,7 +4768,7 @@
       </c>
       <c r="AB10" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -4804,7 +4804,7 @@
       </c>
       <c r="AB11" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -4849,7 +4849,7 @@
       </c>
       <c r="AB12" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>65</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -4882,7 +4882,7 @@
       </c>
       <c r="AB13" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -4927,7 +4927,7 @@
       </c>
       <c r="AB14" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>64</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -4969,7 +4969,7 @@
       </c>
       <c r="AB15" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>61</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -5005,7 +5005,7 @@
       </c>
       <c r="AB16" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -5047,7 +5047,7 @@
       </c>
       <c r="AB17" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -5083,7 +5083,7 @@
       </c>
       <c r="AB18" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -5125,7 +5125,7 @@
       </c>
       <c r="AB19" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="AB20" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5191,7 +5191,7 @@
       </c>
       <c r="AB21" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="AB22" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5254,7 +5254,7 @@
       </c>
       <c r="AB23" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5290,7 +5290,7 @@
       </c>
       <c r="AB24" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5350,7 +5350,7 @@
       </c>
       <c r="AB25" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>97</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5404,7 +5404,7 @@
       </c>
       <c r="AB26" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>89</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5467,7 +5467,7 @@
       </c>
       <c r="AB27" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>99</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5521,7 +5521,7 @@
       </c>
       <c r="AB28" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>68</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5569,7 +5569,7 @@
       </c>
       <c r="AB29" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>51</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5596,7 +5596,7 @@
       </c>
       <c r="AB30" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5635,7 +5635,7 @@
       </c>
       <c r="AB31" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5674,7 +5674,7 @@
       </c>
       <c r="AB32" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>37</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5725,7 +5725,7 @@
       </c>
       <c r="AB33" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>75</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5776,7 +5776,7 @@
       </c>
       <c r="AB34" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>70</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5824,7 +5824,7 @@
       </c>
       <c r="AB35" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>83</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="AB36" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>90</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5935,7 +5935,7 @@
       </c>
       <c r="AB37" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>101</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5974,7 +5974,7 @@
       </c>
       <c r="AB38" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>37</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6025,7 +6025,7 @@
       </c>
       <c r="AB39" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>83</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6070,7 +6070,7 @@
       </c>
       <c r="AB40" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6124,7 +6124,7 @@
       </c>
       <c r="AB41" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>87</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6178,7 +6178,7 @@
       </c>
       <c r="AB42" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>70</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6229,7 +6229,7 @@
       </c>
       <c r="AB43" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6286,7 +6286,7 @@
       </c>
       <c r="AB44" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>78</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6325,7 +6325,7 @@
       </c>
       <c r="AB45" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>42</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6361,7 +6361,7 @@
       </c>
       <c r="AB46" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6406,7 +6406,7 @@
       </c>
       <c r="AB47" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6448,7 +6448,7 @@
       </c>
       <c r="AB48" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6490,7 +6490,7 @@
       </c>
       <c r="AB49" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>50</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6535,7 +6535,7 @@
       </c>
       <c r="AB50" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>63</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6574,7 +6574,7 @@
       </c>
       <c r="AB51" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6619,7 +6619,7 @@
       </c>
       <c r="AB52" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>62</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6664,7 +6664,7 @@
       </c>
       <c r="AB53" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>69</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6694,7 +6694,7 @@
       </c>
       <c r="AB54" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6730,7 +6730,7 @@
       </c>
       <c r="AB55" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6763,7 +6763,7 @@
       </c>
       <c r="AB56" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6811,7 +6811,7 @@
       </c>
       <c r="AB57" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>63</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6850,7 +6850,7 @@
       </c>
       <c r="AB58" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6886,7 +6886,7 @@
       </c>
       <c r="AB59" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6931,7 +6931,7 @@
       </c>
       <c r="AB60" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6967,7 +6967,7 @@
       </c>
       <c r="AB61" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7006,7 +7006,7 @@
       </c>
       <c r="AB62" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7045,7 +7045,7 @@
       </c>
       <c r="AB63" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>64</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7087,7 +7087,7 @@
       </c>
       <c r="AB64" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7141,7 +7141,7 @@
       </c>
       <c r="AB65" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>66</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7180,7 +7180,7 @@
       </c>
       <c r="AB66" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>58</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7234,7 +7234,7 @@
       </c>
       <c r="AB67" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>75</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7285,7 +7285,7 @@
       </c>
       <c r="AB68" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7330,7 +7330,7 @@
       </c>
       <c r="AB69" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>72</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7375,7 +7375,7 @@
       </c>
       <c r="AB70" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7426,7 +7426,7 @@
       </c>
       <c r="AB71" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>64</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7480,7 +7480,7 @@
       </c>
       <c r="AB72" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>71</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7534,7 +7534,7 @@
       </c>
       <c r="AB73" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>79</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7585,7 +7585,7 @@
       </c>
       <c r="AB74" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>66</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7624,7 +7624,7 @@
       </c>
       <c r="AB75" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>58</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7654,7 +7654,7 @@
       </c>
       <c r="AB76" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7674,71 +7674,71 @@
       </c>
       <c r="K79" s="7">
         <f>'Privacy values'!C11</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="L79" s="7">
         <f>'Privacy values'!D11</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="M79" s="7">
         <f>'Privacy values'!E11</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="N79" s="7">
         <f>'Privacy values'!F11</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="O79" s="7">
         <f>'Privacy values'!G11</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="P79" s="7">
         <f>'Privacy values'!H11</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="Q79" s="7">
         <f>'Privacy values'!I11</f>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="R79" s="7">
         <f>'Privacy values'!J11</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S79" s="7">
         <f>'Privacy values'!K11</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="T79" s="7">
         <f>'Privacy values'!L11</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="U79" s="7">
         <f>'Privacy values'!M11</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="V79" s="7">
         <f>'Privacy values'!N11</f>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="W79" s="7">
         <f>'Privacy values'!O11</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="X79" s="7">
         <f>'Privacy values'!P11</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="Y79" s="7">
         <f>'Privacy values'!Q11</f>
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="Z79" s="7">
         <f>'Privacy values'!R11</f>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="AA79" s="7">
         <f>'Privacy values'!S11</f>
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7752,71 +7752,71 @@
       </c>
       <c r="K80" s="7">
         <f>'Privacy values'!C12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L80" s="7">
         <f>'Privacy values'!D12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M80" s="7">
         <f>'Privacy values'!E12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N80" s="7">
         <f>'Privacy values'!F12</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O80" s="7">
         <f>'Privacy values'!G12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P80" s="7">
         <f>'Privacy values'!H12</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Q80" s="7">
         <f>'Privacy values'!I12</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R80" s="7">
         <f>'Privacy values'!J12</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S80" s="7">
         <f>'Privacy values'!K12</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T80" s="7">
         <f>'Privacy values'!L12</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="U80" s="7">
         <f>'Privacy values'!M12</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="V80" s="7">
         <f>'Privacy values'!N12</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="W80" s="7">
         <f>'Privacy values'!O12</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="X80" s="7">
         <f>'Privacy values'!P12</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Y80" s="7">
         <f>'Privacy values'!Q12</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Z80" s="7">
         <f>'Privacy values'!R12</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AA80" s="7">
         <f>'Privacy values'!S12</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="28:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8754,8 +8754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E52125-0BEB-4F52-AF5D-6A00A0E48DCD}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8827,37 +8827,37 @@
         <v>1</v>
       </c>
       <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
       <c r="K2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -8866,16 +8866,16 @@
         <v>1</v>
       </c>
       <c r="P2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>2</v>
       </c>
       <c r="R2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -8892,19 +8892,19 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -8916,25 +8916,25 @@
         <v>1</v>
       </c>
       <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>3</v>
       </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>2</v>
-      </c>
       <c r="R3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -8951,49 +8951,49 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
         <v>2</v>
       </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
+      <c r="N4">
         <v>3</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
       <c r="O4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -9004,10 +9004,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -9019,40 +9019,40 @@
         <v>2</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="R5">
         <v>4</v>
       </c>
-      <c r="R5">
-        <v>2</v>
-      </c>
       <c r="S5">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -9081,7 +9081,7 @@
         <v>2</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -9096,7 +9096,7 @@
         <v>2</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -9105,13 +9105,13 @@
         <v>2</v>
       </c>
       <c r="Q6">
+        <v>6</v>
+      </c>
+      <c r="R6">
         <v>3</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
       <c r="S6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -9122,10 +9122,10 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -9134,13 +9134,13 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -9152,10 +9152,10 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -9164,13 +9164,13 @@
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S7">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -9181,10 +9181,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -9193,28 +9193,28 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -9223,13 +9223,13 @@
         <v>1</v>
       </c>
       <c r="Q8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -9242,10 +9242,10 @@
   <dimension ref="A1:AF989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="J54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I80" sqref="I80:AA80"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35:AF39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9412,19 +9412,19 @@
       </c>
       <c r="AC2" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.666442626740622</v>
+        <v>13.23902800962675</v>
       </c>
       <c r="AD2" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="AE2" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="AF2" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -9475,19 +9475,19 @@
       </c>
       <c r="AC3" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.6266903443929586</v>
+        <v>14.041780843837124</v>
       </c>
       <c r="AD3" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="AE3" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="AF3" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -9529,19 +9529,19 @@
       </c>
       <c r="AC4" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.56235311306681</v>
+        <v>11.90175823201449</v>
       </c>
       <c r="AD4" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="AE4" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="AF4" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -9589,19 +9589,19 @@
       </c>
       <c r="AC5" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>9.7307798580667715</v>
+        <v>15.764336314749816</v>
       </c>
       <c r="AD5" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="AE5" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="AF5" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -9655,19 +9655,19 @@
       </c>
       <c r="AC6" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>9.7307798580667715</v>
+        <v>15.333489185927871</v>
       </c>
       <c r="AD6" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="AE6" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="AF6" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -9721,19 +9721,19 @@
       </c>
       <c r="AC7" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>13.294300065467214</v>
+        <v>20.555315681398646</v>
       </c>
       <c r="AD7" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>100</v>
+        <v>167</v>
       </c>
       <c r="AE7" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="AF7" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -9760,19 +9760,19 @@
       </c>
       <c r="AC8" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>3.9564898674888789</v>
+        <v>6.3655534627892152</v>
       </c>
       <c r="AD8" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="AE8" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AF8" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -9814,19 +9814,19 @@
       </c>
       <c r="AC9" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>10.559211084967036</v>
+        <v>16.49054693928074</v>
       </c>
       <c r="AD9" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="AE9" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="AF9" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
@@ -9853,19 +9853,19 @@
       </c>
       <c r="AC10" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>1.2190136542044754</v>
+        <v>2.0647823694200036</v>
       </c>
       <c r="AD10" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AE10" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AF10" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
@@ -9901,19 +9901,19 @@
       </c>
       <c r="AC11" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>5.1827875340980381</v>
+        <v>7.376004983780577</v>
       </c>
       <c r="AD11" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="AE11" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="AF11" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
@@ -9958,19 +9958,19 @@
       </c>
       <c r="AC12" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.8372085682349493</v>
+        <v>13.598278127980494</v>
       </c>
       <c r="AD12" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="AE12" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="AF12" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
@@ -10003,19 +10003,19 @@
       </c>
       <c r="AC13" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>5.0126374146673962</v>
+        <v>7.0717042989910324</v>
       </c>
       <c r="AD13" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AE13" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="AF13" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
@@ -10060,19 +10060,19 @@
       </c>
       <c r="AC14" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.3583160700240953</v>
+        <v>12.392385554573151</v>
       </c>
       <c r="AD14" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="AE14" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="AF14" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
@@ -10114,19 +10114,19 @@
       </c>
       <c r="AC15" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.088715506615106</v>
+        <v>12.971793238031772</v>
       </c>
       <c r="AD15" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="AE15" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="AF15" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
@@ -10162,19 +10162,19 @@
       </c>
       <c r="AC16" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>3.5421168220827628</v>
+        <v>5.1679380400385631</v>
       </c>
       <c r="AD16" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AE16" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AF16" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
@@ -10216,19 +10216,19 @@
       </c>
       <c r="AC17" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>5.0281111112197117</v>
+        <v>7.376117067386188</v>
       </c>
       <c r="AD17" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="AE17" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AF17" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
@@ -10264,19 +10264,19 @@
       </c>
       <c r="AC18" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>5.0281111112197117</v>
+        <v>7.376117067386188</v>
       </c>
       <c r="AD18" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="AE18" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AF18" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
@@ -10318,19 +10318,19 @@
       </c>
       <c r="AC19" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>6.0281111112197108</v>
+        <v>9.4934168728208572</v>
       </c>
       <c r="AD19" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="AE19" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="AF19" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10366,19 +10366,19 @@
       </c>
       <c r="AC20" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>4.6462063357565748</v>
+        <v>6.8904935109512548</v>
       </c>
       <c r="AD20" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="AE20" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="AF20" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10408,19 +10408,19 @@
       </c>
       <c r="AC21" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>2.3231031678782879</v>
+        <v>3.3564907115107498</v>
       </c>
       <c r="AD21" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="AE21" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AF21" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10450,19 +10450,19 @@
       </c>
       <c r="AC22" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>4.0786980204242269</v>
+        <v>5.6534495128678861</v>
       </c>
       <c r="AD22" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="AE22" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="AF22" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10495,19 +10495,19 @@
       </c>
       <c r="AC23" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>3.5421168220827628</v>
+        <v>5.1679380400385631</v>
       </c>
       <c r="AD23" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AE23" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AF23" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10543,19 +10543,19 @@
       </c>
       <c r="AC24" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>5.7611304762872386</v>
+        <v>7.9810909531074534</v>
       </c>
       <c r="AD24" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="AE24" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="AF24" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10615,19 +10615,19 @@
       </c>
       <c r="AC25" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>13.016484803677889</v>
+        <v>22.248396927026992</v>
       </c>
       <c r="AD25" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>97</v>
+        <v>179</v>
       </c>
       <c r="AE25" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="AF25" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10681,19 +10681,19 @@
       </c>
       <c r="AC26" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>11.846334684247248</v>
+        <v>20.840006728563633</v>
       </c>
       <c r="AD26" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>89</v>
+        <v>168</v>
       </c>
       <c r="AE26" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="AF26" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10756,19 +10756,19 @@
       </c>
       <c r="AC27" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>13.283465438610362</v>
+        <v>23.030414319147237</v>
       </c>
       <c r="AD27" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="AE27" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="AF27" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10822,19 +10822,19 @@
       </c>
       <c r="AC28" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>9.1676350643149895</v>
+        <v>17.456913299103483</v>
       </c>
       <c r="AD28" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="AE28" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="AF28" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10882,19 +10882,19 @@
       </c>
       <c r="AC29" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>6.8445318964367008</v>
+        <v>14.456141557617659</v>
       </c>
       <c r="AD29" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="AE29" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="AF29" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10921,19 +10921,19 @@
       </c>
       <c r="AC30" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>2.7050079433414238</v>
+        <v>4.2729613967676281</v>
       </c>
       <c r="AD30" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="AE30" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AF30" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10972,19 +10972,19 @@
       </c>
       <c r="AC31" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>3.5421168220827628</v>
+        <v>5.1679380400385631</v>
       </c>
       <c r="AD31" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AE31" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AF31" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11023,19 +11023,19 @@
       </c>
       <c r="AC32" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>5.0281111112197117</v>
+        <v>8.3893273591470443</v>
       </c>
       <c r="AD32" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="AE32" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="AF32" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11086,19 +11086,19 @@
       </c>
       <c r="AC33" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>10.029913899030259</v>
+        <v>14.190829367154107</v>
       </c>
       <c r="AD33" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="AE33" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="AF33" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11149,19 +11149,19 @@
       </c>
       <c r="AC34" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>9.3857521644736295</v>
+        <v>15.413940458690984</v>
       </c>
       <c r="AD34" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="AE34" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="AF34" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11209,19 +11209,19 @@
       </c>
       <c r="AC35" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>10.980868142777837</v>
+        <v>16.84160511897343</v>
       </c>
       <c r="AD35" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="AE35" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AF35" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11278,19 +11278,19 @@
       </c>
       <c r="AC36" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>11.980868142777837</v>
+        <v>17.945694632647243</v>
       </c>
       <c r="AD36" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="AE36" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="AF36" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11344,19 +11344,19 @@
       </c>
       <c r="AC37" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>13.466862431914784</v>
+        <v>20.153873659994865</v>
       </c>
       <c r="AD37" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="AE37" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="AF37" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11395,19 +11395,19 @@
       </c>
       <c r="AC38" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>5.0281111112197117</v>
+        <v>8.3893273591470443</v>
       </c>
       <c r="AD38" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="AE38" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="AF38" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11458,19 +11458,19 @@
       </c>
       <c r="AC39" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>10.980868142777837</v>
+        <v>16.84160511897343</v>
       </c>
       <c r="AD39" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="AE39" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AF39" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11515,19 +11515,19 @@
       </c>
       <c r="AC40" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.4781008175258803</v>
+        <v>12.374724017844493</v>
       </c>
       <c r="AD40" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="AE40" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="AF40" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11581,19 +11581,19 @@
       </c>
       <c r="AC41" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>11.708855332351916</v>
+        <v>18.947943258131488</v>
       </c>
       <c r="AD41" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="AE41" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="AF41" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11647,19 +11647,19 @@
       </c>
       <c r="AC42" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>9.207387346662653</v>
+        <v>14.03514989278634</v>
       </c>
       <c r="AD42" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="AE42" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="AF42" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11710,19 +11710,19 @@
       </c>
       <c r="AC43" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.0146820158673435</v>
+        <v>13.057312960312291</v>
       </c>
       <c r="AD43" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="AE43" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="AF43" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11779,19 +11779,19 @@
       </c>
       <c r="AC44" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>10.489841678147441</v>
+        <v>17.136495929603676</v>
       </c>
       <c r="AD44" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="AE44" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="AF44" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11830,19 +11830,19 @@
       </c>
       <c r="AC45" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>5.5646923095611749</v>
+        <v>7.8616285402155111</v>
       </c>
       <c r="AD45" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="AE45" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AF45" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11878,19 +11878,19 @@
       </c>
       <c r="AC46" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>6.6436118672610576</v>
+        <v>10.355662627640879</v>
       </c>
       <c r="AD46" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="AE46" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="AF46" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11935,19 +11935,19 @@
       </c>
       <c r="AC47" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.1393024158196212</v>
+        <v>10.966223919345772</v>
       </c>
       <c r="AD47" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="AE47" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="AF47" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11989,19 +11989,19 @@
       </c>
       <c r="AC48" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.1393024158196212</v>
+        <v>10.966223919345772</v>
       </c>
       <c r="AD48" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="AE48" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="AF48" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12043,19 +12043,19 @@
       </c>
       <c r="AC49" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>6.6027212174781571</v>
+        <v>10.480712446516449</v>
       </c>
       <c r="AD49" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AE49" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="AF49" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12100,19 +12100,19 @@
       </c>
       <c r="AC50" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.2433919294934324</v>
+        <v>12.257932261436519</v>
       </c>
       <c r="AD50" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE50" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="AF50" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12151,19 +12151,19 @@
       </c>
       <c r="AC51" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>6.6687818232349869</v>
+        <v>10.166547174067114</v>
       </c>
       <c r="AD51" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="AE51" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="AF51" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12208,19 +12208,19 @@
       </c>
       <c r="AC52" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.4553037927718115</v>
+        <v>13.112654571545562</v>
       </c>
       <c r="AD52" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="AE52" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="AF52" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12265,19 +12265,19 @@
       </c>
       <c r="AC53" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>9.1928050202889189</v>
+        <v>14.411446944776765</v>
       </c>
       <c r="AD53" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="AE53" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="AF53" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12307,19 +12307,19 @@
       </c>
       <c r="AC54" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>3.5421168220827628</v>
+        <v>5.1679380400385631</v>
       </c>
       <c r="AD54" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AE54" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AF54" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12355,19 +12355,19 @@
       </c>
       <c r="AC55" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>4.6462063357565757</v>
+        <v>7.1733952751189545</v>
       </c>
       <c r="AD55" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="AE55" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="AF55" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12400,19 +12400,19 @@
       </c>
       <c r="AC56" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>3.5421168220827628</v>
+        <v>5.1679380400385631</v>
       </c>
       <c r="AD56" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AE56" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AF56" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12460,19 +12460,19 @@
       </c>
       <c r="AC57" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.2433919294934324</v>
+        <v>12.257932261436519</v>
       </c>
       <c r="AD57" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE57" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="AF57" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12511,19 +12511,19 @@
       </c>
       <c r="AC58" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>6.7573976403564835</v>
+        <v>9.4673900711499801</v>
       </c>
       <c r="AD58" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="AE58" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="AF58" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12559,19 +12559,19 @@
       </c>
       <c r="AC59" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.1393024158196212</v>
+        <v>10.966223919345772</v>
       </c>
       <c r="AD59" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="AE59" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="AF59" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12616,19 +12616,19 @@
       </c>
       <c r="AC60" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>6.7573976403564853</v>
+        <v>9.3194447064957355</v>
       </c>
       <c r="AD60" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="AE60" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="AF60" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12664,19 +12664,19 @@
       </c>
       <c r="AC61" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>5.6533081266826724</v>
+        <v>7.7448346002372901</v>
       </c>
       <c r="AD61" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="AE61" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="AF61" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12715,19 +12715,19 @@
       </c>
       <c r="AC62" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.1393024158196212</v>
+        <v>10.966223919345772</v>
       </c>
       <c r="AD62" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="AE62" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="AF62" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12766,19 +12766,19 @@
       </c>
       <c r="AC63" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.3583160700240953</v>
+        <v>12.392385554573151</v>
       </c>
       <c r="AD63" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="AE63" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="AF63" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12820,19 +12820,19 @@
       </c>
       <c r="AC64" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.5930249580565432</v>
+        <v>12.078330182159178</v>
       </c>
       <c r="AD64" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="AE64" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="AF64" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12886,19 +12886,19 @@
       </c>
       <c r="AC65" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.96409510666283</v>
+        <v>15.448167972298727</v>
       </c>
       <c r="AD65" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="AE65" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="AF65" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12937,19 +12937,19 @@
       </c>
       <c r="AC66" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.8600055929890154</v>
+        <v>14.304404994862228</v>
       </c>
       <c r="AD66" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="AE66" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="AF66" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13003,19 +13003,19 @@
       </c>
       <c r="AC67" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>10.183108760867306</v>
+        <v>17.305176736348052</v>
       </c>
       <c r="AD67" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="AE67" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="AF67" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13066,19 +13066,19 @@
       </c>
       <c r="AC68" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>9.079019247193493</v>
+        <v>15.58262126543536</v>
       </c>
       <c r="AD68" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="AE68" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="AF68" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13123,19 +13123,19 @@
       </c>
       <c r="AC69" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>9.8012039854041682</v>
+        <v>15.375495759330317</v>
       </c>
       <c r="AD69" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="AE69" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="AF69" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13180,19 +13180,19 @@
       </c>
       <c r="AC70" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.5930249580565441</v>
+        <v>12.361231946326878</v>
       </c>
       <c r="AD70" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="AE70" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="AF70" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13243,19 +13243,19 @@
       </c>
       <c r="AC71" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.6971144717303552</v>
+        <v>14.08378741723957</v>
       </c>
       <c r="AD71" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="AE71" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="AF71" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13309,19 +13309,19 @@
       </c>
       <c r="AC72" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>9.5006763050042906</v>
+        <v>15.696339116481862</v>
       </c>
       <c r="AD72" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="AE72" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="AF72" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13375,19 +13375,19 @@
       </c>
       <c r="AC73" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>10.604765818678104</v>
+        <v>17.656234916040741</v>
       </c>
       <c r="AD73" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="AE73" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="AF73" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13438,19 +13438,19 @@
       </c>
       <c r="AC74" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>8.9640951066628283</v>
+        <v>15.879015101120672</v>
       </c>
       <c r="AD74" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="AE74" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="AF74" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13489,19 +13489,19 @@
       </c>
       <c r="AC75" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>7.8600055929890154</v>
+        <v>14.304404994862228</v>
       </c>
       <c r="AD75" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="AE75" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="AF75" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13531,19 +13531,19 @@
       </c>
       <c r="AC76" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$78:$AA$78)</f>
-        <v>3.7839275010413069</v>
+        <v>7.1522811774934283</v>
       </c>
       <c r="AD76" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$79:$AA$79)</f>
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="AE76" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$80:$AA$80)</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AF76" s="4">
         <f>SUMPRODUCT(Table_1[[#This Row],[Nickname]:[Sexual preferences]],$J$81:$AA$81)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13552,19 +13552,19 @@
       </c>
       <c r="AC77" s="9">
         <f>MAX(AC2:AC76)</f>
-        <v>13.466862431914784</v>
+        <v>23.030414319147237</v>
       </c>
       <c r="AD77" s="9">
         <f t="shared" ref="AD77:AF77" si="0">MAX(AD2:AD76)</f>
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="AE77" s="9">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="AF77" s="9">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:32" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13578,90 +13578,90 @@
       </c>
       <c r="K78" s="7">
         <f>'Privacy values'!C10</f>
-        <v>1.2190136542044754</v>
+        <v>1.8114473285278132</v>
       </c>
       <c r="L78" s="7">
         <f>'Privacy values'!D10</f>
-        <v>1.2190136542044754</v>
+        <v>1.8114473285278132</v>
       </c>
       <c r="M78" s="7">
         <f>'Privacy values'!E10</f>
-        <v>1.1040895136738123</v>
+        <v>1.5746101062584457</v>
       </c>
       <c r="N78" s="7">
         <f>'Privacy values'!F10</f>
-        <v>1.2190136542044754</v>
+        <v>1.4261616352273789</v>
       </c>
       <c r="O78" s="7">
         <f>'Privacy values'!G10</f>
-        <v>1.4859942891369484</v>
+        <v>2.2081790273476245</v>
       </c>
       <c r="P78" s="7">
         <f>'Privacy values'!H10</f>
-        <v>1.2190136542044754</v>
+        <v>2.0647823694200036</v>
       </c>
       <c r="Q78" s="7">
         <f>'Privacy values'!I10</f>
-        <v>1.4859942891369484</v>
+        <v>3.2213893191084817</v>
       </c>
       <c r="R78" s="7">
         <f>'Privacy values'!J10</f>
-        <v>1</v>
+        <v>1.1040895136738123</v>
       </c>
       <c r="S78" s="7">
         <f>'Privacy values'!K10</f>
-        <v>1.1040895136738123</v>
+        <v>1.7225554709126913</v>
       </c>
       <c r="T78" s="7">
         <f>'Privacy values'!L10</f>
-        <v>1.5746101062584457</v>
+        <v>2.0913850873694031</v>
       </c>
       <c r="U78" s="7">
         <f>'Privacy values'!M10</f>
-        <v>1.5746101062584457</v>
+        <v>2.9946807841156105</v>
       </c>
       <c r="V78" s="7">
         <f>'Privacy values'!N10</f>
-        <v>1.3459001926323562</v>
+        <v>3.2760514795456119</v>
       </c>
       <c r="W78" s="7">
         <f>'Privacy values'!O10</f>
-        <v>1.1040895136738123</v>
+        <v>1.2917083420907465</v>
       </c>
       <c r="X78" s="7">
         <f>'Privacy values'!P10</f>
-        <v>1.6406707120152757</v>
+        <v>1.7772198149200693</v>
       </c>
       <c r="Y78" s="7">
         <f>'Privacy values'!Q10</f>
-        <v>2.7374762132844035</v>
+        <v>4.300771093369212</v>
       </c>
       <c r="Z78" s="7">
         <f>'Privacy values'!R10</f>
-        <v>1.5746101062584457</v>
+        <v>4.082471061015748</v>
       </c>
       <c r="AA78" s="7">
         <f>'Privacy values'!S10</f>
-        <v>2.379565578968772</v>
+        <v>4.9566003770558593</v>
       </c>
       <c r="AB78" t="s">
         <v>234</v>
       </c>
       <c r="AC78" s="9">
         <f>MIN(AC2:AC76)</f>
-        <v>1.2190136542044754</v>
+        <v>2.0647823694200036</v>
       </c>
       <c r="AD78" s="9">
         <f t="shared" ref="AD78:AF78" si="1">MIN(AD2:AD76)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AE78" s="9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AF78" s="9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:32" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13675,90 +13675,90 @@
       </c>
       <c r="K79" s="7">
         <f>'Privacy values'!C11</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="L79" s="7">
         <f>'Privacy values'!D11</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="M79" s="7">
         <f>'Privacy values'!E11</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="N79" s="7">
         <f>'Privacy values'!F11</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="O79" s="7">
         <f>'Privacy values'!G11</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="P79" s="7">
         <f>'Privacy values'!H11</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="Q79" s="7">
         <f>'Privacy values'!I11</f>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="R79" s="7">
         <f>'Privacy values'!J11</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S79" s="7">
         <f>'Privacy values'!K11</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="T79" s="7">
         <f>'Privacy values'!L11</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="U79" s="7">
         <f>'Privacy values'!M11</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="V79" s="7">
         <f>'Privacy values'!N11</f>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="W79" s="7">
         <f>'Privacy values'!O11</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="X79" s="7">
         <f>'Privacy values'!P11</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="Y79" s="7">
         <f>'Privacy values'!Q11</f>
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="Z79" s="7">
         <f>'Privacy values'!R11</f>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="AA79" s="7">
         <f>'Privacy values'!S11</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="AB79" t="s">
         <v>26</v>
       </c>
       <c r="AC79" s="9">
         <f>GEOMEAN(AC2:AC76)</f>
-        <v>7.0051105610094488</v>
+        <v>11.009469060681214</v>
       </c>
       <c r="AD79" s="9">
         <f t="shared" ref="AD79:AF79" si="2">GEOMEAN(AD2:AD76)</f>
-        <v>52.286969945621912</v>
+        <v>89.098817628330281</v>
       </c>
       <c r="AE79" s="9">
         <f t="shared" si="2"/>
-        <v>12.068861269491313</v>
+        <v>27.028995936490325</v>
       </c>
       <c r="AF79" s="9">
         <f t="shared" si="2"/>
-        <v>6.7264063004347427</v>
+        <v>9.7063514033144198</v>
       </c>
     </row>
     <row r="80" spans="1:32" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13772,90 +13772,90 @@
       </c>
       <c r="K80" s="7">
         <f>'Privacy values'!C12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L80" s="7">
         <f>'Privacy values'!D12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M80" s="7">
         <f>'Privacy values'!E12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N80" s="7">
         <f>'Privacy values'!F12</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O80" s="7">
         <f>'Privacy values'!G12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P80" s="7">
         <f>'Privacy values'!H12</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Q80" s="7">
         <f>'Privacy values'!I12</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R80" s="7">
         <f>'Privacy values'!J12</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S80" s="7">
         <f>'Privacy values'!K12</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T80" s="7">
         <f>'Privacy values'!L12</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="U80" s="7">
         <f>'Privacy values'!M12</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="V80" s="7">
         <f>'Privacy values'!N12</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="W80" s="7">
         <f>'Privacy values'!O12</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="X80" s="7">
         <f>'Privacy values'!P12</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Y80" s="7">
         <f>'Privacy values'!Q12</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Z80" s="7">
         <f>'Privacy values'!R12</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AA80" s="7">
         <f>'Privacy values'!S12</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AB80" t="s">
         <v>233</v>
       </c>
       <c r="AC80" s="9">
         <f>MEDIAN(AC5:AC79)</f>
-        <v>7.5930249580565441</v>
+        <v>12.361231946326878</v>
       </c>
       <c r="AD80" s="9">
         <f t="shared" ref="AD80:AF80" si="3">MEDIAN(AD5:AD79)</f>
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="AE80" s="9">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="AF80" s="9">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="9:32" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13869,11 +13869,11 @@
       </c>
       <c r="K81" s="7">
         <f>'Privacy values'!C13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L81" s="7">
         <f>'Privacy values'!D13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M81" s="7">
         <f>'Privacy values'!E13</f>
@@ -13889,11 +13889,11 @@
       </c>
       <c r="P81" s="7">
         <f>'Privacy values'!H13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q81" s="7">
         <f>'Privacy values'!I13</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R81" s="7">
         <f>'Privacy values'!J13</f>
@@ -13909,11 +13909,11 @@
       </c>
       <c r="U81" s="7">
         <f>'Privacy values'!M13</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V81" s="7">
         <f>'Privacy values'!N13</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W81" s="7">
         <f>'Privacy values'!O13</f>
@@ -13921,38 +13921,38 @@
       </c>
       <c r="X81" s="7">
         <f>'Privacy values'!P13</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y81" s="7">
         <f>'Privacy values'!Q13</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z81" s="7">
         <f>'Privacy values'!R13</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA81" s="7">
         <f>'Privacy values'!S13</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB81" t="s">
         <v>235</v>
       </c>
       <c r="AC81" s="9">
         <f>_xlfn.STDEV.P(AC6:AC80)</f>
-        <v>2.9348849365101399</v>
+        <v>4.9970108801642246</v>
       </c>
       <c r="AD81" s="9">
         <f t="shared" ref="AD81:AF81" si="4">_xlfn.STDEV.P(AD6:AD80)</f>
-        <v>22.034778230727433</v>
+        <v>40.052470475767883</v>
       </c>
       <c r="AE81" s="9">
         <f t="shared" si="4"/>
-        <v>5.1775469626384893</v>
+        <v>11.124720561049914</v>
       </c>
       <c r="AF81" s="9">
         <f t="shared" si="4"/>
-        <v>3.0917587614646056</v>
+        <v>4.3529460894314527</v>
       </c>
     </row>
     <row r="82" spans="9:32" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -13962,19 +13962,19 @@
       </c>
       <c r="AC83" s="11">
         <f>SUM(J78:AA78)</f>
-        <v>25.987754751789382</v>
+        <v>42.715550138486314</v>
       </c>
       <c r="AD83" s="11">
         <f>SUM(J79:AA79)</f>
-        <v>194</v>
+        <v>337</v>
       </c>
       <c r="AE83" s="11">
         <f>SUM(J80:AA80)</f>
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="AF83" s="11">
         <f>SUM(J81:AA81)</f>
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84" spans="9:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13993,7 +13993,7 @@
         <v>241</v>
       </c>
       <c r="AD87" s="4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="9:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14001,7 +14001,7 @@
         <v>240</v>
       </c>
       <c r="AD88" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="9:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14009,7 +14009,7 @@
         <v>242</v>
       </c>
       <c r="AD89" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="9:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14017,7 +14017,7 @@
         <v>243</v>
       </c>
       <c r="AD90" s="12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="9:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14025,12 +14025,12 @@
         <v>244</v>
       </c>
       <c r="AD91" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="9:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB92" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="AD92" s="4" t="s">
         <v>251</v>
@@ -15014,6 +15014,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -15084,37 +15085,37 @@
         <v>1</v>
       </c>
       <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
       <c r="K2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -15123,16 +15124,16 @@
         <v>1</v>
       </c>
       <c r="P2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>2</v>
       </c>
       <c r="R2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -15149,19 +15150,19 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -15173,25 +15174,25 @@
         <v>1</v>
       </c>
       <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>3</v>
       </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>2</v>
-      </c>
       <c r="R3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -15208,49 +15209,49 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
         <v>2</v>
       </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
+      <c r="N4">
         <v>3</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
       <c r="O4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -15261,10 +15262,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -15276,40 +15277,40 @@
         <v>2</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="R5">
         <v>4</v>
       </c>
-      <c r="R5">
-        <v>2</v>
-      </c>
       <c r="S5">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -15338,7 +15339,7 @@
         <v>2</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -15353,7 +15354,7 @@
         <v>2</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -15362,13 +15363,13 @@
         <v>2</v>
       </c>
       <c r="Q6">
+        <v>6</v>
+      </c>
+      <c r="R6">
         <v>3</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
       <c r="S6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -15379,10 +15380,10 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -15391,13 +15392,13 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -15409,10 +15410,10 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -15421,13 +15422,13 @@
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S7">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -15438,10 +15439,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -15450,28 +15451,28 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -15480,13 +15481,13 @@
         <v>1</v>
       </c>
       <c r="Q8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -15504,75 +15505,75 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" ref="C10:S10" si="0">GEOMEAN(C2:C8)</f>
-        <v>1.2190136542044754</v>
+        <v>1.8114473285278132</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>1.2190136542044754</v>
+        <v>1.8114473285278132</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>1.1040895136738123</v>
+        <v>1.5746101062584457</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
-        <v>1.2190136542044754</v>
+        <v>1.4261616352273789</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>1.4859942891369484</v>
+        <v>2.2081790273476245</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="0"/>
-        <v>1.2190136542044754</v>
+        <v>2.0647823694200036</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>1.4859942891369484</v>
+        <v>3.2213893191084817</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.1040895136738123</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="0"/>
-        <v>1.1040895136738123</v>
+        <v>1.7225554709126913</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" si="0"/>
-        <v>1.5746101062584457</v>
+        <v>2.0913850873694031</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>1.5746101062584457</v>
+        <v>2.9946807841156105</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="0"/>
-        <v>1.3459001926323562</v>
+        <v>3.2760514795456119</v>
       </c>
       <c r="O10" s="3">
         <f t="shared" si="0"/>
-        <v>1.1040895136738123</v>
+        <v>1.2917083420907465</v>
       </c>
       <c r="P10" s="3">
         <f t="shared" si="0"/>
-        <v>1.6406707120152757</v>
+        <v>1.7772198149200693</v>
       </c>
       <c r="Q10" s="3">
         <f t="shared" si="0"/>
-        <v>2.7374762132844035</v>
+        <v>4.300771093369212</v>
       </c>
       <c r="R10" s="3">
         <f t="shared" si="0"/>
-        <v>1.5746101062584457</v>
+        <v>4.082471061015748</v>
       </c>
       <c r="S10" s="3">
         <f t="shared" si="0"/>
-        <v>2.379565578968772</v>
+        <v>4.9566003770558593</v>
       </c>
       <c r="T10" s="3">
         <f>SUM(B10:S10)</f>
-        <v>25.987754751789382</v>
+        <v>42.715550138486314</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -15585,75 +15586,75 @@
       </c>
       <c r="C11">
         <f t="shared" ref="C11:S11" si="1">SUM(C2:C8)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N11">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="O11">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="P11">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="Q11">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="R11">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="T11" s="3">
         <f t="shared" ref="T11:T13" si="2">SUM(B11:S11)</f>
-        <v>194</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -15666,75 +15667,75 @@
       </c>
       <c r="C12">
         <f t="shared" ref="C12:S12" si="3">MAX(C2:C8)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J12">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M12">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N12">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P12">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q12">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R12">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S12">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="T12" s="3">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -15747,11 +15748,11 @@
       </c>
       <c r="C13">
         <f t="shared" ref="C13:S13" si="4">MEDIAN(C2:C8)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <f t="shared" si="4"/>
@@ -15767,11 +15768,11 @@
       </c>
       <c r="H13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13">
         <f t="shared" si="4"/>
@@ -15787,11 +15788,11 @@
       </c>
       <c r="M13">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O13">
         <f t="shared" si="4"/>
@@ -15799,23 +15800,23 @@
       </c>
       <c r="P13">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R13">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S13">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T13" s="3">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
NIST compliance added and small changes
</commit_message>
<xml_diff>
--- a/services/risk_dimensions.xlsx
+++ b/services/risk_dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roise\Documents\Apam ciber\leaks\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56794841-BC05-4908-A3CF-BB1D16A8A7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9B869F-ED4E-428F-A153-90FB4CD11E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="6240" windowWidth="20880" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Services clean" sheetId="4" r:id="rId1"/>
@@ -19,10 +19,10 @@
     <sheet name="Privacy values" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Services test'!$AG$2:$AG$75</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Services test'!$AF$2:$AF$75</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Services test'!$AD$2:$AD$75</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Services test'!$AG$2:$AG$75</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Services test'!$AE$2:$AE$75</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Services test'!$AD$2:$AD$75</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Services test'!$AF$2:$AF$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -755,22 +755,22 @@
     <t>gog.com</t>
   </si>
   <si>
-    <t>250-</t>
-  </si>
-  <si>
-    <t>0-50</t>
-  </si>
-  <si>
-    <t>50-100</t>
-  </si>
-  <si>
-    <t>100-150</t>
-  </si>
-  <si>
-    <t>150-200</t>
-  </si>
-  <si>
-    <t>200-250</t>
+    <t>0-30</t>
+  </si>
+  <si>
+    <t>30-60</t>
+  </si>
+  <si>
+    <t>60-90</t>
+  </si>
+  <si>
+    <t>90-120</t>
+  </si>
+  <si>
+    <t>120-150</t>
+  </si>
+  <si>
+    <t>150-</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1336,7 +1336,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1397,7 +1397,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4305,11 +4305,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C522F9-F455-4B38-A565-C6DB8983C156}">
   <dimension ref="A1:AF987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB81" sqref="AB81"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10438,11 +10438,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F9EBD0-2CFC-417B-A678-6B092CE088D1}">
   <dimension ref="A1:AI988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH74" sqref="AH74"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16368,7 +16368,7 @@
         <v>226</v>
       </c>
       <c r="AE86" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="87" spans="28:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -16376,7 +16376,7 @@
         <v>225</v>
       </c>
       <c r="AE87" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" spans="28:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -16384,7 +16384,7 @@
         <v>227</v>
       </c>
       <c r="AE88" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="89" spans="28:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -16392,7 +16392,7 @@
         <v>228</v>
       </c>
       <c r="AE89" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="90" spans="28:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -16400,7 +16400,7 @@
         <v>229</v>
       </c>
       <c r="AE90" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="28:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -16408,7 +16408,7 @@
         <v>230</v>
       </c>
       <c r="AE91" s="13" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="92" spans="28:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
risk dimensions test update
</commit_message>
<xml_diff>
--- a/services/risk_dimensions.xlsx
+++ b/services/risk_dimensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roise\Documents\Apam ciber\leaks\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147B9913-924B-4FC9-91CA-C1AED4D34E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7F362B-2E12-4E1C-90C8-B981C1DF5CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,10 @@
     <sheet name="Privacy values" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Services sum test'!$AF$2:$AF$75</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Services sum test'!$AE$2:$AE$75</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Services sum test'!$AG$2:$AG$75</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Services sum test'!$AD$2:$AD$75</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Services risk test'!$AF$2:$AF$75</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Services risk test'!$AG$2:$AG$75</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Services sum test'!$AG$2:$AG$75</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Services sum test'!$AF$2:$AF$75</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Services sum test'!$AD$2:$AD$75</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Services sum test'!$AE$2:$AE$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="245">
   <si>
     <t>Nickname</t>
   </si>
@@ -778,6 +776,12 @@
   <si>
     <t>S</t>
   </si>
+  <si>
+    <t>sum(RxD)/7</t>
+  </si>
+  <si>
+    <t>1/S*(sum(RxD)/7)</t>
+  </si>
 </sst>
 </file>
 
@@ -1340,7 +1344,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1401,7 +1405,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1462,7 +1466,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1523,7 +1527,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -17545,13 +17549,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F696BBE8-A62F-4829-97BF-9BE9B83C6F20}">
-  <dimension ref="A1:AL988"/>
+  <dimension ref="A1:AO988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL2" sqref="AL2:AL75"/>
+      <selection pane="bottomRight" activeCell="AO8" sqref="AO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17579,7 +17583,7 @@
     <col min="36" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>27</v>
       </c>
@@ -17685,11 +17689,18 @@
       <c r="AJ1" t="s">
         <v>24</v>
       </c>
+      <c r="AK1" s="3"/>
       <c r="AL1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AM1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>35</v>
       </c>
@@ -17734,6 +17745,7 @@
       <c r="AB2" s="11">
         <v>1</v>
       </c>
+      <c r="AC2" s="3"/>
       <c r="AD2" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>16</v>
@@ -17764,11 +17776,22 @@
       </c>
       <c r="AK2" s="3"/>
       <c r="AL2">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM2">
+        <f>SUM(AD2:AJ2)/7</f>
+        <v>16.857142857142858</v>
+      </c>
+      <c r="AN2">
+        <f>AM2/AL2</f>
+        <v>11.238095238095239</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>39</v>
       </c>
@@ -17814,6 +17837,7 @@
       <c r="AB3" s="11">
         <v>1</v>
       </c>
+      <c r="AC3" s="3"/>
       <c r="AD3" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>20</v>
@@ -17843,11 +17867,19 @@
         <v>15</v>
       </c>
       <c r="AL3">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" ref="AM3:AM66" si="0">SUM(AD3:AJ3)/7</f>
+        <v>15.571428571428571</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" ref="AN3:AN66" si="1">AM3/AL3</f>
+        <v>18.685714285714287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
@@ -17894,6 +17926,7 @@
       <c r="AB4" s="11">
         <v>1</v>
       </c>
+      <c r="AC4" s="3"/>
       <c r="AD4" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>12</v>
@@ -17923,11 +17956,19 @@
         <v>14</v>
       </c>
       <c r="AL4">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" si="0"/>
+        <v>15.428571428571429</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" si="1"/>
+        <v>12.342857142857143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -17972,6 +18013,7 @@
       <c r="AB5" s="11">
         <v>1</v>
       </c>
+      <c r="AC5" s="3"/>
       <c r="AD5" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>24</v>
@@ -18001,11 +18043,19 @@
         <v>19</v>
       </c>
       <c r="AL5">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="0"/>
+        <v>18.428571428571427</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="1"/>
+        <v>36.857142857142854</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -18055,6 +18105,7 @@
       <c r="AB6" s="11">
         <v>1</v>
       </c>
+      <c r="AC6" s="3"/>
       <c r="AD6" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>18</v>
@@ -18084,11 +18135,19 @@
         <v>15</v>
       </c>
       <c r="AL6">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" si="0"/>
+        <v>16.428571428571427</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" si="1"/>
+        <v>10.952380952380951</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -18142,6 +18201,7 @@
       </c>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
+      <c r="AC7" s="3"/>
       <c r="AD7" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>36</v>
@@ -18171,11 +18231,19 @@
         <v>18</v>
       </c>
       <c r="AL7">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.7499999999999998</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" si="0"/>
+        <v>25.857142857142858</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" si="1"/>
+        <v>14.775510204081634</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -18200,6 +18268,7 @@
       </c>
       <c r="AA8" s="11"/>
       <c r="AB8" s="11"/>
+      <c r="AC8" s="3"/>
       <c r="AD8" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>3</v>
@@ -18229,11 +18298,19 @@
         <v>8</v>
       </c>
       <c r="AL8">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -18273,6 +18350,7 @@
       </c>
       <c r="AA9" s="11"/>
       <c r="AB9" s="11"/>
+      <c r="AC9" s="3"/>
       <c r="AD9" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>26</v>
@@ -18302,11 +18380,19 @@
         <v>15</v>
       </c>
       <c r="AL9">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="1"/>
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -18336,6 +18422,7 @@
       </c>
       <c r="AA10" s="11"/>
       <c r="AB10" s="11"/>
+      <c r="AC10" s="3"/>
       <c r="AD10" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>9</v>
@@ -18365,11 +18452,19 @@
         <v>6</v>
       </c>
       <c r="AL10">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="0"/>
+        <v>6.5714285714285712</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="1"/>
+        <v>6.5714285714285712</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -18402,6 +18497,7 @@
       </c>
       <c r="AA11" s="11"/>
       <c r="AB11" s="11"/>
+      <c r="AC11" s="3"/>
       <c r="AD11" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>8</v>
@@ -18431,11 +18527,19 @@
         <v>7</v>
       </c>
       <c r="AL11">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM11">
+        <f t="shared" si="0"/>
+        <v>7.8571428571428568</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="1"/>
+        <v>7.8571428571428568</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -18480,6 +18584,7 @@
       </c>
       <c r="AA12" s="11"/>
       <c r="AB12" s="11"/>
+      <c r="AC12" s="3"/>
       <c r="AD12" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>26</v>
@@ -18509,11 +18614,19 @@
         <v>13</v>
       </c>
       <c r="AL12">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>2</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="0"/>
+        <v>17.428571428571427</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="1"/>
+        <v>8.7142857142857135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -18547,6 +18660,7 @@
       </c>
       <c r="AA13" s="11"/>
       <c r="AB13" s="11"/>
+      <c r="AC13" s="3"/>
       <c r="AD13" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>18</v>
@@ -18576,11 +18690,19 @@
         <v>8</v>
       </c>
       <c r="AL13">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="AM13">
+        <f t="shared" si="0"/>
+        <v>10.428571428571429</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="1"/>
+        <v>8.9387755102040831</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -18628,6 +18750,7 @@
       </c>
       <c r="AA14" s="11"/>
       <c r="AB14" s="11"/>
+      <c r="AC14" s="3"/>
       <c r="AD14" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>26</v>
@@ -18657,11 +18780,19 @@
         <v>12</v>
       </c>
       <c r="AL14">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM14">
+        <f t="shared" si="0"/>
+        <v>17.857142857142858</v>
+      </c>
+      <c r="AN14">
+        <f t="shared" si="1"/>
+        <v>14.285714285714286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -18706,6 +18837,7 @@
       </c>
       <c r="AA15" s="11"/>
       <c r="AB15" s="11"/>
+      <c r="AC15" s="3"/>
       <c r="AD15" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>30</v>
@@ -18735,11 +18867,19 @@
         <v>13</v>
       </c>
       <c r="AL15">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM15">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -18775,6 +18915,7 @@
       </c>
       <c r="AA16" s="11"/>
       <c r="AB16" s="11"/>
+      <c r="AC16" s="3"/>
       <c r="AD16" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>7</v>
@@ -18804,11 +18945,19 @@
         <v>6</v>
       </c>
       <c r="AL16">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM16">
+        <f t="shared" si="0"/>
+        <v>7.4285714285714288</v>
+      </c>
+      <c r="AN16">
+        <f t="shared" si="1"/>
+        <v>4.9523809523809526</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -18847,6 +18996,7 @@
       </c>
       <c r="AA17" s="11"/>
       <c r="AB17" s="11"/>
+      <c r="AC17" s="3"/>
       <c r="AD17" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>14</v>
@@ -18876,11 +19026,19 @@
         <v>9</v>
       </c>
       <c r="AL17">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>2</v>
+      </c>
+      <c r="AM17">
+        <f t="shared" si="0"/>
+        <v>10.428571428571429</v>
+      </c>
+      <c r="AN17">
+        <f t="shared" si="1"/>
+        <v>5.2142857142857144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -18916,6 +19074,7 @@
       </c>
       <c r="AA18" s="11"/>
       <c r="AB18" s="11"/>
+      <c r="AC18" s="3"/>
       <c r="AD18" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>14</v>
@@ -18945,11 +19104,19 @@
         <v>9</v>
       </c>
       <c r="AL18">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.75</v>
+      </c>
+      <c r="AM18">
+        <f t="shared" si="0"/>
+        <v>10.428571428571429</v>
+      </c>
+      <c r="AN18">
+        <f t="shared" si="1"/>
+        <v>13.904761904761905</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -18997,6 +19164,7 @@
       </c>
       <c r="AA19" s="11"/>
       <c r="AB19" s="11"/>
+      <c r="AC19" s="3"/>
       <c r="AD19" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>21</v>
@@ -19026,11 +19194,19 @@
         <v>12</v>
       </c>
       <c r="AL19">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM19">
+        <f t="shared" si="0"/>
+        <v>15.142857142857142</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" si="1"/>
+        <v>12.114285714285714</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -19066,6 +19242,7 @@
       </c>
       <c r="AA20" s="11"/>
       <c r="AB20" s="11"/>
+      <c r="AC20" s="3"/>
       <c r="AD20" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>15</v>
@@ -19095,11 +19272,19 @@
         <v>10</v>
       </c>
       <c r="AL20">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM20">
+        <f t="shared" si="0"/>
+        <v>10.285714285714286</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" si="1"/>
+        <v>10.285714285714286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -19136,6 +19321,7 @@
       </c>
       <c r="AA21" s="11"/>
       <c r="AB21" s="11"/>
+      <c r="AC21" s="3"/>
       <c r="AD21" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>7</v>
@@ -19165,11 +19351,19 @@
         <v>6</v>
       </c>
       <c r="AL21">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM21">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="AN21">
+        <f t="shared" si="1"/>
+        <v>7.1428571428571432</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -19194,6 +19388,7 @@
       </c>
       <c r="AA22" s="11"/>
       <c r="AB22" s="11"/>
+      <c r="AC22" s="3"/>
       <c r="AD22" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>2</v>
@@ -19223,11 +19418,19 @@
         <v>3</v>
       </c>
       <c r="AL22">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM22">
+        <f t="shared" si="0"/>
+        <v>4.7142857142857144</v>
+      </c>
+      <c r="AN22">
+        <f t="shared" si="1"/>
+        <v>7.0714285714285721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -19263,6 +19466,7 @@
       </c>
       <c r="AA23" s="11"/>
       <c r="AB23" s="11"/>
+      <c r="AC23" s="3"/>
       <c r="AD23" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>14</v>
@@ -19292,11 +19496,19 @@
         <v>9</v>
       </c>
       <c r="AL23">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM23">
+        <f t="shared" si="0"/>
+        <v>10.428571428571429</v>
+      </c>
+      <c r="AN23">
+        <f t="shared" si="1"/>
+        <v>10.428571428571429</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -19330,6 +19542,7 @@
       </c>
       <c r="AA24" s="11"/>
       <c r="AB24" s="11"/>
+      <c r="AC24" s="3"/>
       <c r="AD24" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>11</v>
@@ -19359,11 +19572,19 @@
         <v>6</v>
       </c>
       <c r="AL24">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM24">
+        <f t="shared" si="0"/>
+        <v>7.8571428571428568</v>
+      </c>
+      <c r="AN24">
+        <f t="shared" si="1"/>
+        <v>11.785714285714286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -19422,6 +19643,7 @@
         <v>1</v>
       </c>
       <c r="AB25" s="11"/>
+      <c r="AC25" s="3"/>
       <c r="AD25" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>36</v>
@@ -19451,11 +19673,19 @@
         <v>25</v>
       </c>
       <c r="AL25">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AN25">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -19508,6 +19738,7 @@
         <v>1</v>
       </c>
       <c r="AB26" s="11"/>
+      <c r="AC26" s="3"/>
       <c r="AD26" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>33</v>
@@ -19537,11 +19768,19 @@
         <v>20</v>
       </c>
       <c r="AL26">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM26">
+        <f t="shared" si="0"/>
+        <v>26.142857142857142</v>
+      </c>
+      <c r="AN26">
+        <f t="shared" si="1"/>
+        <v>17.428571428571427</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -19600,6 +19839,7 @@
         <v>1</v>
       </c>
       <c r="AB27" s="11"/>
+      <c r="AC27" s="3"/>
       <c r="AD27" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>33</v>
@@ -19629,11 +19869,19 @@
         <v>24</v>
       </c>
       <c r="AL27">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM27">
+        <f t="shared" si="0"/>
+        <v>28.428571428571427</v>
+      </c>
+      <c r="AN27">
+        <f t="shared" si="1"/>
+        <v>22.74285714285714</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -19683,6 +19931,7 @@
         <v>1</v>
       </c>
       <c r="AB28" s="11"/>
+      <c r="AC28" s="3"/>
       <c r="AD28" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>25</v>
@@ -19712,11 +19961,19 @@
         <v>18</v>
       </c>
       <c r="AL28">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM28">
+        <f t="shared" si="0"/>
+        <v>21.285714285714285</v>
+      </c>
+      <c r="AN28">
+        <f t="shared" si="1"/>
+        <v>14.19047619047619</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -19760,6 +20017,7 @@
         <v>1</v>
       </c>
       <c r="AB29" s="11"/>
+      <c r="AC29" s="3"/>
       <c r="AD29" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>18</v>
@@ -19789,11 +20047,19 @@
         <v>16</v>
       </c>
       <c r="AL29">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM29">
+        <f t="shared" si="0"/>
+        <v>17.857142857142858</v>
+      </c>
+      <c r="AN29">
+        <f t="shared" si="1"/>
+        <v>17.857142857142858</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>107</v>
       </c>
@@ -19821,6 +20087,7 @@
       </c>
       <c r="AA30" s="11"/>
       <c r="AB30" s="11"/>
+      <c r="AC30" s="3"/>
       <c r="AD30" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>6</v>
@@ -19850,11 +20117,19 @@
         <v>5</v>
       </c>
       <c r="AL30">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM30">
+        <f t="shared" si="0"/>
+        <v>5.5714285714285712</v>
+      </c>
+      <c r="AN30">
+        <f t="shared" si="1"/>
+        <v>8.3571428571428577</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -19888,6 +20163,7 @@
       </c>
       <c r="AA31" s="11"/>
       <c r="AB31" s="11"/>
+      <c r="AC31" s="3"/>
       <c r="AD31" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>3</v>
@@ -19917,11 +20193,19 @@
         <v>4</v>
       </c>
       <c r="AL31">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM31">
+        <f t="shared" si="0"/>
+        <v>5.1428571428571432</v>
+      </c>
+      <c r="AN31">
+        <f t="shared" si="1"/>
+        <v>3.4285714285714288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -19955,6 +20239,7 @@
       </c>
       <c r="AA32" s="11"/>
       <c r="AB32" s="11"/>
+      <c r="AC32" s="3"/>
       <c r="AD32" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>8</v>
@@ -19984,11 +20269,19 @@
         <v>6</v>
       </c>
       <c r="AL32">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM32">
+        <f t="shared" si="0"/>
+        <v>8.7142857142857135</v>
+      </c>
+      <c r="AN32">
+        <f t="shared" si="1"/>
+        <v>13.071428571428571</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -20034,6 +20327,7 @@
       </c>
       <c r="AA33" s="11"/>
       <c r="AB33" s="11"/>
+      <c r="AC33" s="3"/>
       <c r="AD33" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>26</v>
@@ -20063,11 +20357,19 @@
         <v>12</v>
       </c>
       <c r="AL33">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="AM33">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="AN33">
+        <f t="shared" si="1"/>
+        <v>13.714285714285715</v>
+      </c>
+    </row>
+    <row r="34" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -20115,6 +20417,7 @@
       </c>
       <c r="AA34" s="11"/>
       <c r="AB34" s="11"/>
+      <c r="AC34" s="3"/>
       <c r="AD34" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>18</v>
@@ -20144,11 +20447,19 @@
         <v>13</v>
       </c>
       <c r="AL34">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM34">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AN34">
+        <f t="shared" si="1"/>
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -20193,6 +20504,7 @@
       </c>
       <c r="AA35" s="11"/>
       <c r="AB35" s="11"/>
+      <c r="AC35" s="3"/>
       <c r="AD35" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>28</v>
@@ -20222,11 +20534,19 @@
         <v>17</v>
       </c>
       <c r="AL35">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM35">
+        <f t="shared" si="0"/>
+        <v>21.857142857142858</v>
+      </c>
+      <c r="AN35">
+        <f t="shared" si="1"/>
+        <v>21.857142857142858</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>124</v>
       </c>
@@ -20280,6 +20600,7 @@
       </c>
       <c r="AA36" s="11"/>
       <c r="AB36" s="11"/>
+      <c r="AC36" s="3"/>
       <c r="AD36" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>30</v>
@@ -20309,11 +20630,19 @@
         <v>18</v>
       </c>
       <c r="AL36">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM36">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AN36">
+        <f t="shared" si="1"/>
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>127</v>
       </c>
@@ -20370,6 +20699,7 @@
       </c>
       <c r="AA37" s="11"/>
       <c r="AB37" s="11"/>
+      <c r="AC37" s="3"/>
       <c r="AD37" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>34</v>
@@ -20399,11 +20729,19 @@
         <v>20</v>
       </c>
       <c r="AL37">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM37">
+        <f t="shared" si="0"/>
+        <v>25.285714285714285</v>
+      </c>
+      <c r="AN37">
+        <f t="shared" si="1"/>
+        <v>20.228571428571428</v>
+      </c>
+    </row>
+    <row r="38" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>129</v>
       </c>
@@ -20448,6 +20786,7 @@
       </c>
       <c r="AA38" s="11"/>
       <c r="AB38" s="11"/>
+      <c r="AC38" s="3"/>
       <c r="AD38" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>16</v>
@@ -20477,11 +20816,19 @@
         <v>10</v>
       </c>
       <c r="AL38">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM38">
+        <f t="shared" si="0"/>
+        <v>12.714285714285714</v>
+      </c>
+      <c r="AN38">
+        <f t="shared" si="1"/>
+        <v>12.714285714285714</v>
+      </c>
+    </row>
+    <row r="39" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>131</v>
       </c>
@@ -20529,6 +20876,7 @@
       </c>
       <c r="AA39" s="11"/>
       <c r="AB39" s="11"/>
+      <c r="AC39" s="3"/>
       <c r="AD39" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>28</v>
@@ -20558,11 +20906,19 @@
         <v>17</v>
       </c>
       <c r="AL39">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM39">
+        <f t="shared" si="0"/>
+        <v>21.857142857142858</v>
+      </c>
+      <c r="AN39">
+        <f t="shared" si="1"/>
+        <v>17.485714285714288</v>
+      </c>
+    </row>
+    <row r="40" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -20611,6 +20967,7 @@
       </c>
       <c r="AA40" s="11"/>
       <c r="AB40" s="11"/>
+      <c r="AC40" s="3"/>
       <c r="AD40" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>21</v>
@@ -20640,11 +20997,19 @@
         <v>16</v>
       </c>
       <c r="AL40">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM40">
+        <f t="shared" si="0"/>
+        <v>17.285714285714285</v>
+      </c>
+      <c r="AN40">
+        <f t="shared" si="1"/>
+        <v>25.928571428571427</v>
+      </c>
+    </row>
+    <row r="41" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>135</v>
       </c>
@@ -20696,6 +21061,7 @@
       </c>
       <c r="AA41" s="11"/>
       <c r="AB41" s="11"/>
+      <c r="AC41" s="3"/>
       <c r="AD41" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>26</v>
@@ -20725,11 +21091,19 @@
         <v>17</v>
       </c>
       <c r="AL41">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM41">
+        <f t="shared" si="0"/>
+        <v>22.142857142857142</v>
+      </c>
+      <c r="AN41">
+        <f t="shared" si="1"/>
+        <v>33.214285714285715</v>
+      </c>
+    </row>
+    <row r="42" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>138</v>
       </c>
@@ -20783,6 +21157,7 @@
       </c>
       <c r="AA42" s="11"/>
       <c r="AB42" s="11"/>
+      <c r="AC42" s="3"/>
       <c r="AD42" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>25</v>
@@ -20812,11 +21187,19 @@
         <v>16</v>
       </c>
       <c r="AL42">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM42">
+        <f t="shared" si="0"/>
+        <v>20.428571428571427</v>
+      </c>
+      <c r="AN42">
+        <f t="shared" si="1"/>
+        <v>20.428571428571427</v>
+      </c>
+    </row>
+    <row r="43" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>141</v>
       </c>
@@ -20870,6 +21253,7 @@
       </c>
       <c r="AA43" s="11"/>
       <c r="AB43" s="11"/>
+      <c r="AC43" s="3"/>
       <c r="AD43" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>13</v>
@@ -20899,11 +21283,19 @@
         <v>11</v>
       </c>
       <c r="AL43">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM43">
+        <f t="shared" si="0"/>
+        <v>16.428571428571427</v>
+      </c>
+      <c r="AN43">
+        <f t="shared" si="1"/>
+        <v>10.952380952380951</v>
+      </c>
+    </row>
+    <row r="44" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>144</v>
       </c>
@@ -20960,6 +21352,7 @@
       </c>
       <c r="AA44" s="11"/>
       <c r="AB44" s="11"/>
+      <c r="AC44" s="3"/>
       <c r="AD44" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>27</v>
@@ -20989,11 +21382,19 @@
         <v>18</v>
       </c>
       <c r="AL44">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM44">
+        <f t="shared" si="0"/>
+        <v>23.142857142857142</v>
+      </c>
+      <c r="AN44">
+        <f t="shared" si="1"/>
+        <v>15.428571428571429</v>
+      </c>
+    </row>
+    <row r="45" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>146</v>
       </c>
@@ -21035,6 +21436,7 @@
       </c>
       <c r="AA45" s="11"/>
       <c r="AB45" s="11"/>
+      <c r="AC45" s="3"/>
       <c r="AD45" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>16</v>
@@ -21064,11 +21466,19 @@
         <v>10</v>
       </c>
       <c r="AL45">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM45">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AN45">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -21105,6 +21515,7 @@
       </c>
       <c r="AA46" s="11"/>
       <c r="AB46" s="11"/>
+      <c r="AC46" s="3"/>
       <c r="AD46" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>14</v>
@@ -21134,11 +21545,19 @@
         <v>11</v>
       </c>
       <c r="AL46">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM46">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AN46">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>149</v>
       </c>
@@ -21186,6 +21605,7 @@
       </c>
       <c r="AA47" s="11"/>
       <c r="AB47" s="11"/>
+      <c r="AC47" s="3"/>
       <c r="AD47" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>23</v>
@@ -21215,11 +21635,19 @@
         <v>11</v>
       </c>
       <c r="AL47">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM47">
+        <f t="shared" si="0"/>
+        <v>16.285714285714285</v>
+      </c>
+      <c r="AN47">
+        <f t="shared" si="1"/>
+        <v>16.285714285714285</v>
+      </c>
+    </row>
+    <row r="48" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>153</v>
       </c>
@@ -21267,6 +21695,7 @@
       </c>
       <c r="AA48" s="11"/>
       <c r="AB48" s="11"/>
+      <c r="AC48" s="3"/>
       <c r="AD48" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>23</v>
@@ -21296,11 +21725,19 @@
         <v>11</v>
       </c>
       <c r="AL48">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>2</v>
+      </c>
+      <c r="AM48">
+        <f t="shared" si="0"/>
+        <v>16.285714285714285</v>
+      </c>
+      <c r="AN48">
+        <f t="shared" si="1"/>
+        <v>8.1428571428571423</v>
+      </c>
+    </row>
+    <row r="49" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>156</v>
       </c>
@@ -21342,6 +21779,7 @@
       </c>
       <c r="AA49" s="11"/>
       <c r="AB49" s="11"/>
+      <c r="AC49" s="3"/>
       <c r="AD49" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>22</v>
@@ -21371,11 +21809,19 @@
         <v>10</v>
       </c>
       <c r="AL49">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM49">
+        <f t="shared" si="0"/>
+        <v>14.714285714285714</v>
+      </c>
+      <c r="AN49">
+        <f t="shared" si="1"/>
+        <v>9.8095238095238084</v>
+      </c>
+    </row>
+    <row r="50" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>158</v>
       </c>
@@ -21423,6 +21869,7 @@
       </c>
       <c r="AA50" s="11"/>
       <c r="AB50" s="11"/>
+      <c r="AC50" s="3"/>
       <c r="AD50" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>23</v>
@@ -21452,11 +21899,19 @@
         <v>11</v>
       </c>
       <c r="AL50">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM50">
+        <f t="shared" si="0"/>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="AN50">
+        <f t="shared" si="1"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>160</v>
       </c>
@@ -21498,6 +21953,7 @@
       </c>
       <c r="AA51" s="11"/>
       <c r="AB51" s="11"/>
+      <c r="AC51" s="3"/>
       <c r="AD51" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>20</v>
@@ -21527,11 +21983,19 @@
         <v>12</v>
       </c>
       <c r="AL51">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM51">
+        <f t="shared" si="0"/>
+        <v>16.428571428571427</v>
+      </c>
+      <c r="AN51">
+        <f t="shared" si="1"/>
+        <v>16.428571428571427</v>
+      </c>
+    </row>
+    <row r="52" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>162</v>
       </c>
@@ -21579,6 +22043,7 @@
       </c>
       <c r="AA52" s="11"/>
       <c r="AB52" s="11"/>
+      <c r="AC52" s="3"/>
       <c r="AD52" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>31</v>
@@ -21608,11 +22073,19 @@
         <v>16</v>
       </c>
       <c r="AL52">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM52">
+        <f t="shared" si="0"/>
+        <v>19.571428571428573</v>
+      </c>
+      <c r="AN52">
+        <f t="shared" si="1"/>
+        <v>15.657142857142858</v>
+      </c>
+    </row>
+    <row r="53" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>165</v>
       </c>
@@ -21655,6 +22128,7 @@
       </c>
       <c r="AA53" s="11"/>
       <c r="AB53" s="11"/>
+      <c r="AC53" s="3"/>
       <c r="AD53" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>24</v>
@@ -21684,11 +22158,19 @@
         <v>12</v>
       </c>
       <c r="AL53">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM53">
+        <f t="shared" si="0"/>
+        <v>16.142857142857142</v>
+      </c>
+      <c r="AN53">
+        <f t="shared" si="1"/>
+        <v>16.142857142857142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>167</v>
       </c>
@@ -21725,6 +22207,7 @@
       </c>
       <c r="AA54" s="11"/>
       <c r="AB54" s="11"/>
+      <c r="AC54" s="3"/>
       <c r="AD54" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>15</v>
@@ -21754,11 +22237,19 @@
         <v>10</v>
       </c>
       <c r="AL54">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM54">
+        <f t="shared" si="0"/>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="AN54">
+        <f t="shared" si="1"/>
+        <v>17.142857142857146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>169</v>
       </c>
@@ -21789,6 +22280,7 @@
       </c>
       <c r="AA55" s="11"/>
       <c r="AB55" s="11"/>
+      <c r="AC55" s="3"/>
       <c r="AD55" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>11</v>
@@ -21818,11 +22310,19 @@
         <v>7</v>
       </c>
       <c r="AL55">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM55">
+        <f t="shared" si="0"/>
+        <v>7.2857142857142856</v>
+      </c>
+      <c r="AN55">
+        <f t="shared" si="1"/>
+        <v>10.928571428571429</v>
+      </c>
+    </row>
+    <row r="56" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>171</v>
       </c>
@@ -21859,6 +22359,7 @@
       </c>
       <c r="AA56" s="11"/>
       <c r="AB56" s="11"/>
+      <c r="AC56" s="3"/>
       <c r="AD56" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>16</v>
@@ -21888,11 +22389,19 @@
         <v>11</v>
       </c>
       <c r="AL56">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM56">
+        <f t="shared" si="0"/>
+        <v>11.285714285714286</v>
+      </c>
+      <c r="AN56">
+        <f t="shared" si="1"/>
+        <v>16.928571428571431</v>
+      </c>
+    </row>
+    <row r="57" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>173</v>
       </c>
@@ -21940,6 +22449,7 @@
       </c>
       <c r="AA57" s="11"/>
       <c r="AB57" s="11"/>
+      <c r="AC57" s="3"/>
       <c r="AD57" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>23</v>
@@ -21969,11 +22479,19 @@
         <v>11</v>
       </c>
       <c r="AL57">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM57">
+        <f t="shared" si="0"/>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="AN57">
+        <f t="shared" si="1"/>
+        <v>17.142857142857142</v>
+      </c>
+    </row>
+    <row r="58" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>176</v>
       </c>
@@ -22009,6 +22527,7 @@
       </c>
       <c r="AA58" s="11"/>
       <c r="AB58" s="11"/>
+      <c r="AC58" s="3"/>
       <c r="AD58" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>18</v>
@@ -22038,11 +22557,19 @@
         <v>9</v>
       </c>
       <c r="AL58">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM58">
+        <f t="shared" si="0"/>
+        <v>11.857142857142858</v>
+      </c>
+      <c r="AN58">
+        <f t="shared" si="1"/>
+        <v>11.857142857142858</v>
+      </c>
+    </row>
+    <row r="59" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>178</v>
       </c>
@@ -22079,6 +22606,7 @@
       </c>
       <c r="AA59" s="11"/>
       <c r="AB59" s="11"/>
+      <c r="AC59" s="3"/>
       <c r="AD59" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>22</v>
@@ -22108,11 +22636,19 @@
         <v>10</v>
       </c>
       <c r="AL59">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM59">
+        <f t="shared" si="0"/>
+        <v>15.285714285714286</v>
+      </c>
+      <c r="AN59">
+        <f t="shared" si="1"/>
+        <v>22.928571428571431</v>
+      </c>
+    </row>
+    <row r="60" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>180</v>
       </c>
@@ -22155,6 +22691,7 @@
       </c>
       <c r="AA60" s="11"/>
       <c r="AB60" s="11"/>
+      <c r="AC60" s="3"/>
       <c r="AD60" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>21</v>
@@ -22184,11 +22721,19 @@
         <v>9</v>
       </c>
       <c r="AL60">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="AM60">
+        <f t="shared" si="0"/>
+        <v>13.571428571428571</v>
+      </c>
+      <c r="AN60">
+        <f t="shared" si="1"/>
+        <v>16.285714285714288</v>
+      </c>
+    </row>
+    <row r="61" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>182</v>
       </c>
@@ -22227,6 +22772,7 @@
       </c>
       <c r="AA61" s="11"/>
       <c r="AB61" s="11"/>
+      <c r="AC61" s="3"/>
       <c r="AD61" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>17</v>
@@ -22256,11 +22802,19 @@
         <v>8</v>
       </c>
       <c r="AL61">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.25</v>
+      </c>
+      <c r="AM61">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AN61">
+        <f t="shared" si="1"/>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>184</v>
       </c>
@@ -22299,6 +22853,7 @@
       </c>
       <c r="AA62" s="11"/>
       <c r="AB62" s="11"/>
+      <c r="AC62" s="3"/>
       <c r="AD62" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>22</v>
@@ -22328,11 +22883,19 @@
         <v>10</v>
       </c>
       <c r="AL62">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.75</v>
+      </c>
+      <c r="AM62">
+        <f t="shared" si="0"/>
+        <v>15.285714285714286</v>
+      </c>
+      <c r="AN62">
+        <f t="shared" si="1"/>
+        <v>20.380952380952383</v>
+      </c>
+    </row>
+    <row r="63" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>186</v>
       </c>
@@ -22372,6 +22935,7 @@
       </c>
       <c r="AA63" s="11"/>
       <c r="AB63" s="11"/>
+      <c r="AC63" s="3"/>
       <c r="AD63" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>18</v>
@@ -22401,11 +22965,19 @@
         <v>8</v>
       </c>
       <c r="AL63">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM63">
+        <f t="shared" si="0"/>
+        <v>13.857142857142858</v>
+      </c>
+      <c r="AN63">
+        <f t="shared" si="1"/>
+        <v>20.785714285714288</v>
+      </c>
+    </row>
+    <row r="64" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>188</v>
       </c>
@@ -22453,6 +23025,7 @@
       </c>
       <c r="AA64" s="11"/>
       <c r="AB64" s="11"/>
+      <c r="AC64" s="3"/>
       <c r="AD64" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>23</v>
@@ -22482,11 +23055,19 @@
         <v>16</v>
       </c>
       <c r="AL64">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM64">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AN64">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>190</v>
       </c>
@@ -22537,6 +23118,7 @@
       </c>
       <c r="AA65" s="11"/>
       <c r="AB65" s="11"/>
+      <c r="AC65" s="3"/>
       <c r="AD65" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>17</v>
@@ -22566,11 +23148,19 @@
         <v>12</v>
       </c>
       <c r="AL65">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM65">
+        <f t="shared" si="0"/>
+        <v>16.571428571428573</v>
+      </c>
+      <c r="AN65">
+        <f t="shared" si="1"/>
+        <v>11.047619047619049</v>
+      </c>
+    </row>
+    <row r="66" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>193</v>
       </c>
@@ -22610,6 +23200,7 @@
       </c>
       <c r="AA66" s="11"/>
       <c r="AB66" s="11"/>
+      <c r="AC66" s="3"/>
       <c r="AD66" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>22</v>
@@ -22639,11 +23230,19 @@
         <v>16</v>
       </c>
       <c r="AL66">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM66">
+        <f t="shared" si="0"/>
+        <v>18.285714285714285</v>
+      </c>
+      <c r="AN66">
+        <f t="shared" si="1"/>
+        <v>27.428571428571427</v>
+      </c>
+    </row>
+    <row r="67" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>195</v>
       </c>
@@ -22700,6 +23299,7 @@
       </c>
       <c r="AA67" s="11"/>
       <c r="AB67" s="11"/>
+      <c r="AC67" s="3"/>
       <c r="AD67" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>36</v>
@@ -22729,11 +23329,19 @@
         <v>21</v>
       </c>
       <c r="AL67">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.75</v>
+      </c>
+      <c r="AM67">
+        <f t="shared" ref="AM67:AM75" si="2">SUM(AD67:AJ67)/7</f>
+        <v>24.714285714285715</v>
+      </c>
+      <c r="AN67">
+        <f t="shared" ref="AN67:AN75" si="3">AM67/AL67</f>
+        <v>32.952380952380956</v>
+      </c>
+    </row>
+    <row r="68" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>198</v>
       </c>
@@ -22787,6 +23395,7 @@
       </c>
       <c r="AA68" s="11"/>
       <c r="AB68" s="11"/>
+      <c r="AC68" s="3"/>
       <c r="AD68" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>24</v>
@@ -22816,11 +23425,19 @@
         <v>15</v>
       </c>
       <c r="AL68">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.75</v>
+      </c>
+      <c r="AM68">
+        <f t="shared" si="2"/>
+        <v>19.571428571428573</v>
+      </c>
+      <c r="AN68">
+        <f t="shared" si="3"/>
+        <v>26.095238095238098</v>
+      </c>
+    </row>
+    <row r="69" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>200</v>
       </c>
@@ -22869,6 +23486,7 @@
       </c>
       <c r="AA69" s="11"/>
       <c r="AB69" s="11"/>
+      <c r="AC69" s="3"/>
       <c r="AD69" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>32</v>
@@ -22898,11 +23516,19 @@
         <v>20</v>
       </c>
       <c r="AL69">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM69">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="AN69">
+        <f t="shared" si="3"/>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>202</v>
       </c>
@@ -22956,6 +23582,7 @@
       </c>
       <c r="AA70" s="11"/>
       <c r="AB70" s="11"/>
+      <c r="AC70" s="3"/>
       <c r="AD70" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>27</v>
@@ -22985,11 +23612,19 @@
         <v>17</v>
       </c>
       <c r="AL70">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM70">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="AN70">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>204</v>
       </c>
@@ -23043,6 +23678,7 @@
       </c>
       <c r="AA71" s="11"/>
       <c r="AB71" s="11"/>
+      <c r="AC71" s="3"/>
       <c r="AD71" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>32</v>
@@ -23072,11 +23708,19 @@
         <v>20</v>
       </c>
       <c r="AL71">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM71">
+        <f t="shared" si="2"/>
+        <v>22.142857142857142</v>
+      </c>
+      <c r="AN71">
+        <f t="shared" si="3"/>
+        <v>22.142857142857142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>206</v>
       </c>
@@ -23127,6 +23771,7 @@
       </c>
       <c r="AA72" s="11"/>
       <c r="AB72" s="11"/>
+      <c r="AC72" s="3"/>
       <c r="AD72" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>26</v>
@@ -23156,11 +23801,19 @@
         <v>18</v>
       </c>
       <c r="AL72">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="AM72">
+        <f t="shared" si="2"/>
+        <v>22.285714285714285</v>
+      </c>
+      <c r="AN72">
+        <f t="shared" si="3"/>
+        <v>14.857142857142856</v>
+      </c>
+    </row>
+    <row r="73" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>208</v>
       </c>
@@ -23208,6 +23861,7 @@
       </c>
       <c r="AA73" s="11"/>
       <c r="AB73" s="11"/>
+      <c r="AC73" s="3"/>
       <c r="AD73" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>27</v>
@@ -23237,11 +23891,19 @@
         <v>18</v>
       </c>
       <c r="AL73">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM73">
+        <f t="shared" si="2"/>
+        <v>22.571428571428573</v>
+      </c>
+      <c r="AN73">
+        <f t="shared" si="3"/>
+        <v>22.571428571428573</v>
+      </c>
+    </row>
+    <row r="74" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>211</v>
       </c>
@@ -23295,6 +23957,7 @@
       </c>
       <c r="AA74" s="11"/>
       <c r="AB74" s="11"/>
+      <c r="AC74" s="3"/>
       <c r="AD74" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>26</v>
@@ -23324,11 +23987,19 @@
         <v>17</v>
       </c>
       <c r="AL74">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM74">
+        <f t="shared" si="2"/>
+        <v>20.142857142857142</v>
+      </c>
+      <c r="AN74">
+        <f t="shared" si="3"/>
+        <v>20.142857142857142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>214</v>
       </c>
@@ -23361,6 +24032,7 @@
       </c>
       <c r="AA75" s="11"/>
       <c r="AB75" s="11"/>
+      <c r="AC75" s="3"/>
       <c r="AD75" s="3">
         <f>SUMPRODUCT(Table_14[[#This Row],[Nickname]:[Sexual preferences]],'privacy values clean'!$B$2:$S$2)</f>
         <v>12</v>
@@ -23390,11 +24062,19 @@
         <v>11</v>
       </c>
       <c r="AL75">
-        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+Table_14[[#This Row],[min length]])/10))</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(((IF(Table_14[[#This Row],[extra sec]]=1,1,0)+IF(Table_14[[#This Row],[min mask]]="l",1,0)+IF(Table_14[[#This Row],[min length]]&gt;7,1,0))/6+0.5)+IF(Table_14[[#This Row],[min length]]&gt;8,0.5,0))*IF(Table_14[[#This Row],[2fa]]=1,1.5,1)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AM75">
+        <f t="shared" si="2"/>
+        <v>12.571428571428571</v>
+      </c>
+      <c r="AN75">
+        <f t="shared" si="3"/>
+        <v>18.857142857142858</v>
+      </c>
+    </row>
+    <row r="76" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -23419,7 +24099,7 @@
       <c r="X76" s="3"/>
       <c r="Y76" s="3"/>
     </row>
-    <row r="77" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -23505,7 +24185,7 @@
         <v>5.1496638245683073</v>
       </c>
     </row>
-    <row r="78" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -23591,7 +24271,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -23677,7 +24357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -24696,6 +25376,30 @@
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <conditionalFormatting sqref="AM2:AM75">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN2:AN75">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>